<commit_message>
CMA Compliance sw SOS completeness
</commit_message>
<xml_diff>
--- a/Projects/CCBOTTLERSUS/CMA_SOUTHWEST/Data/Southwest CMA Compliance Template_v4.xlsx
+++ b/Projects/CCBOTTLERSUS/CMA_SOUTHWEST/Data/Southwest CMA Compliance Template_v4.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="112">
   <si>
     <t>KPI name</t>
   </si>
@@ -157,28 +157,6 @@
     <t>att4</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Energy </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>KO</t>
-    </r>
-  </si>
-  <si>
     <t>brand_name</t>
   </si>
   <si>
@@ -243,9 +221,6 @@
   </si>
   <si>
     <t>SHELF STABLE PROTEIN</t>
-  </si>
-  <si>
-    <t>Client Subcategory Name</t>
   </si>
   <si>
     <t>POWERADE</t>
@@ -422,19 +397,6 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="7"/>
       <color rgb="FF333333"/>
       <name val="Arial"/>
@@ -465,6 +427,13 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -475,6 +444,12 @@
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -626,7 +601,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="24">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -650,24 +625,12 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="44">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -680,7 +643,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -692,47 +655,39 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="21" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="23" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -744,43 +699,43 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="23" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="23" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="23" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="23" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="23" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="23" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -800,7 +755,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="23" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -816,7 +771,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -832,46 +787,35 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="10">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Explanatory Text 2" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Normal 2" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Normal 3" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Normal 4" xfId="23" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -943,14 +887,14 @@
   </sheetPr>
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.9595141700405"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.5425101214575"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.8178137651822"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.8178137651822"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.10526315789474"/>
@@ -1116,7 +1060,7 @@
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="4" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="4" width="42.5263157894737"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="4" width="42.9554655870445"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="4" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="1013" min="4" style="4" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1022" min="1014" style="5" width="9.10526315789474"/>
@@ -1164,23 +1108,23 @@
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
+      <selection pane="topLeft" activeCell="B43" activeCellId="0" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.9595141700405"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.3522267206478"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.9595141700405"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="17.995951417004"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="42.5263157894737"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.8542510121457"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="42.5263157894737"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="28.2793522267206"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="34.8137651821862"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="21.1012145748988"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="18.3157894736842"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.2105263157895"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.1740890688259"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.4615384615385"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.1740890688259"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="18.1012145748988"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="42.9554655870445"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="42.9554655870445"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="28.4939271255061"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="35.0283400809717"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="21.2105263157895"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.3198380566802"/>
     <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1276,67 +1220,67 @@
     </row>
     <row r="4" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="C4" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="13" t="s">
         <v>40</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>37</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L4" s="0" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="13" t="s">
+    <row r="5" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D5" s="14" t="s">
+      <c r="B5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="13" t="s">
         <v>40</v>
       </c>
       <c r="F5" s="0"/>
       <c r="G5" s="0"/>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="I5" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="L5" s="13" t="s">
+      <c r="I5" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="L5" s="2" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="16" t="s">
-        <v>48</v>
+      <c r="A6" s="14" t="s">
+        <v>47</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="17" t="s">
-        <v>49</v>
+      <c r="C6" s="15" t="s">
+        <v>48</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>39</v>
@@ -1347,19 +1291,19 @@
       <c r="H6" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="I6" s="17" t="s">
+      <c r="I6" s="15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="14" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="16" t="s">
-        <v>50</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="17" t="s">
-        <v>50</v>
+      <c r="C7" s="15" t="s">
+        <v>49</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>39</v>
@@ -1370,19 +1314,19 @@
       <c r="H7" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="I7" s="17" t="s">
+      <c r="I7" s="15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="14" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="16" t="s">
-        <v>51</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="17" t="s">
-        <v>52</v>
+      <c r="C8" s="15" t="s">
+        <v>51</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>39</v>
@@ -1393,42 +1337,42 @@
       <c r="H8" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="I8" s="17" t="s">
+      <c r="I8" s="15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="14" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="16" t="s">
+      <c r="B9" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="C9" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="13" t="s">
         <v>40</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="I9" s="17" t="s">
-        <v>50</v>
+      <c r="I9" s="15" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="16" t="s">
-        <v>56</v>
+      <c r="A10" s="14" t="s">
+        <v>55</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>39</v>
@@ -1440,7 +1384,7 @@
         <v>37</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1461,17 +1405,17 @@
   </sheetPr>
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H19" activeCellId="0" sqref="H19"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.9595141700405"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.3157894736842"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.6356275303644"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.8502024291498"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.10526315789474"/>
   </cols>
@@ -1481,45 +1425,45 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="E1" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="F1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2"/>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="H1" s="2"/>
-    </row>
-    <row r="2" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="D2" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="E2" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="13" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1527,16 +1471,16 @@
       <c r="A3" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="D3" s="14" t="s">
+      <c r="B3" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="13" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1547,19 +1491,19 @@
       <c r="B4" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="D4" s="19" t="s">
-        <v>66</v>
+      <c r="C4" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>53</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="F4" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="13" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1568,15 +1512,15 @@
         <v>15</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="D5" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="13" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1585,21 +1529,21 @@
         <v>17</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="F6" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F6" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="G6" s="13" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1608,15 +1552,15 @@
         <v>18</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="D7" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="13" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1639,12 +1583,12 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.5303643724696"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.6396761133603"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.21052631578947"/>
   </cols>
   <sheetData>
@@ -1653,16 +1597,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="E1" s="0" t="s">
         <v>59</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1689,16 +1633,16 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.4251012145749"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.2793522267206"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.5303643724696"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.4939271255061"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.3562753036437"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.1740890688259"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="35.0283400809717"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.3846153846154"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="35.2429149797571"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1710,16 +1654,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="F1" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1729,13 +1673,13 @@
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="D2" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="F2" s="23" t="n">
+      <c r="C2" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="F2" s="22" t="n">
         <v>0.4</v>
       </c>
     </row>
@@ -1746,13 +1690,13 @@
       <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="D3" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="F3" s="23" t="n">
+      <c r="C3" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="F3" s="22" t="n">
         <v>0.45</v>
       </c>
     </row>
@@ -1763,14 +1707,14 @@
       <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="F4" s="23" t="s">
         <v>75</v>
-      </c>
-      <c r="D4" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="F4" s="24" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1780,14 +1724,14 @@
       <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="F5" s="23" t="s">
         <v>75</v>
-      </c>
-      <c r="D5" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="F5" s="24" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1797,14 +1741,14 @@
       <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="D6" s="22" t="s">
+      <c r="C6" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="F6" s="23" t="s">
         <v>76</v>
-      </c>
-      <c r="F6" s="24" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1814,14 +1758,14 @@
       <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="D7" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="F7" s="24" t="s">
-        <v>79</v>
+      <c r="C7" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="F7" s="23" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1831,14 +1775,14 @@
       <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="D8" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="F8" s="24" t="s">
-        <v>80</v>
+      <c r="C8" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1848,14 +1792,14 @@
       <c r="B9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="D9" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="F9" s="24" t="s">
-        <v>81</v>
+      <c r="C9" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="F9" s="23" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1865,14 +1809,14 @@
       <c r="B10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="D10" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="F10" s="24" t="s">
-        <v>82</v>
+      <c r="C10" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="F10" s="23" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1882,14 +1826,14 @@
       <c r="B11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="D11" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="F11" s="24" t="s">
-        <v>83</v>
+      <c r="C11" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="F11" s="23" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1899,14 +1843,14 @@
       <c r="B12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="D12" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="F12" s="24" t="s">
-        <v>84</v>
+      <c r="C12" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="F12" s="23" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1916,13 +1860,13 @@
       <c r="B13" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="D13" s="25" t="s">
-        <v>85</v>
-      </c>
-      <c r="F13" s="26" t="n">
+      <c r="C13" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="F13" s="24" t="n">
         <v>0.38</v>
       </c>
     </row>
@@ -1933,98 +1877,98 @@
       <c r="B14" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="D14" s="25" t="s">
-        <v>85</v>
-      </c>
-      <c r="F14" s="26" t="n">
+      <c r="C14" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="F14" s="24" t="n">
         <v>0.15</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="27" t="s">
-        <v>48</v>
+      <c r="A15" s="25" t="s">
+        <v>47</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="D15" s="25" t="s">
-        <v>85</v>
-      </c>
-      <c r="F15" s="28" t="n">
+      <c r="C15" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="F15" s="26" t="n">
         <v>0.3</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="27" t="s">
-        <v>50</v>
+      <c r="A16" s="25" t="s">
+        <v>49</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="D16" s="25" t="s">
-        <v>85</v>
-      </c>
-      <c r="F16" s="28" t="n">
+      <c r="C16" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="F16" s="26" t="n">
         <v>0.33</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="27" t="s">
-        <v>51</v>
+      <c r="A17" s="25" t="s">
+        <v>50</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="D17" s="25" t="s">
-        <v>85</v>
-      </c>
-      <c r="F17" s="28" t="n">
+      <c r="C17" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="F17" s="26" t="n">
         <v>0.15</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="27" t="s">
-        <v>53</v>
+      <c r="A18" s="25" t="s">
+        <v>52</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="D18" s="25" t="s">
-        <v>85</v>
-      </c>
-      <c r="F18" s="28" t="n">
+      <c r="C18" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="F18" s="26" t="n">
         <v>0.5</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="27" t="s">
-        <v>56</v>
+      <c r="A19" s="25" t="s">
+        <v>55</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="D19" s="25" t="s">
-        <v>85</v>
-      </c>
-      <c r="F19" s="28" t="n">
+      <c r="C19" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="F19" s="26" t="n">
         <v>0.2</v>
       </c>
     </row>
@@ -2052,342 +1996,342 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.2834008097166"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.6720647773279"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.8866396761134"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.5708502024291"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.7085020242915"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.1740890688259"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="10.0688259109312"/>
-    <col collapsed="false" hidden="false" max="14" min="9" style="0" width="9.63967611336032"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.9230769230769"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.3846153846154"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="10.1781376518219"/>
+    <col collapsed="false" hidden="false" max="14" min="9" style="0" width="9.74898785425101"/>
     <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G1" s="29" t="s">
+      <c r="G1" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>60</v>
-      </c>
       <c r="F2" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="G2" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="G2" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="H2" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="I2" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="H2" s="31" t="s">
+      <c r="J2" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="I2" s="31" t="s">
+      <c r="K2" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="J2" s="31" t="s">
+      <c r="L2" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="K2" s="31" t="s">
+      <c r="M2" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="L2" s="31" t="s">
+      <c r="N2" s="30" t="s">
         <v>91</v>
-      </c>
-      <c r="M2" s="31" t="s">
-        <v>92</v>
-      </c>
-      <c r="N2" s="32" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C3" s="11" t="s">
+      <c r="E3" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="D3" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="F3" s="33" t="s">
-        <v>85</v>
-      </c>
-      <c r="G3" s="34" t="n">
+      <c r="F3" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="G3" s="32" t="n">
         <v>2</v>
       </c>
-      <c r="H3" s="35" t="n">
+      <c r="H3" s="33" t="n">
         <v>2</v>
       </c>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35"/>
-      <c r="L3" s="35"/>
-      <c r="M3" s="35"/>
-      <c r="N3" s="36"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="33"/>
+      <c r="K3" s="33"/>
+      <c r="L3" s="33"/>
+      <c r="M3" s="33"/>
+      <c r="N3" s="34"/>
     </row>
     <row r="4" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" s="35" t="s">
         <v>98</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C4" s="37" t="s">
-        <v>100</v>
-      </c>
-      <c r="F4" s="33" t="s">
-        <v>85</v>
-      </c>
-      <c r="G4" s="38" t="n">
+      <c r="F4" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="G4" s="36" t="n">
         <v>2</v>
       </c>
-      <c r="H4" s="39" t="n">
+      <c r="H4" s="37" t="n">
         <v>3</v>
       </c>
-      <c r="I4" s="39"/>
-      <c r="J4" s="39"/>
-      <c r="K4" s="39"/>
-      <c r="L4" s="39"/>
-      <c r="M4" s="39"/>
-      <c r="N4" s="40"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="37"/>
+      <c r="M4" s="37"/>
+      <c r="N4" s="38"/>
     </row>
     <row r="5" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="F5" s="33" t="s">
-        <v>85</v>
-      </c>
-      <c r="G5" s="38"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="39" t="n">
+        <v>100</v>
+      </c>
+      <c r="F5" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="G5" s="36"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37" t="n">
         <v>1</v>
       </c>
-      <c r="J5" s="39" t="n">
+      <c r="J5" s="37" t="n">
         <v>1</v>
       </c>
-      <c r="K5" s="39" t="n">
+      <c r="K5" s="37" t="n">
         <v>2</v>
       </c>
-      <c r="L5" s="39" t="n">
+      <c r="L5" s="37" t="n">
         <v>2</v>
       </c>
-      <c r="M5" s="39" t="n">
+      <c r="M5" s="37" t="n">
         <v>2</v>
       </c>
-      <c r="N5" s="40" t="n">
+      <c r="N5" s="38" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="43" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C6" s="41" t="s">
-        <v>104</v>
-      </c>
-      <c r="D6" s="13"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="33" t="s">
-        <v>85</v>
-      </c>
-      <c r="G6" s="38"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39" t="n">
+        <v>97</v>
+      </c>
+      <c r="C6" s="39" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="G6" s="36"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37" t="n">
         <v>1</v>
       </c>
-      <c r="J6" s="39" t="n">
+      <c r="J6" s="37" t="n">
         <v>1</v>
       </c>
-      <c r="K6" s="39" t="n">
+      <c r="K6" s="37" t="n">
         <v>3</v>
       </c>
-      <c r="L6" s="39" t="n">
+      <c r="L6" s="37" t="n">
         <v>3</v>
       </c>
-      <c r="M6" s="39" t="n">
+      <c r="M6" s="37" t="n">
         <v>3</v>
       </c>
-      <c r="N6" s="40" t="n">
+      <c r="N6" s="38" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="53.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C7" s="41" t="s">
-        <v>106</v>
-      </c>
-      <c r="F7" s="33" t="s">
-        <v>85</v>
-      </c>
-      <c r="G7" s="38"/>
-      <c r="H7" s="39"/>
-      <c r="I7" s="39"/>
-      <c r="J7" s="39"/>
-      <c r="K7" s="39" t="n">
+        <v>97</v>
+      </c>
+      <c r="C7" s="39" t="s">
+        <v>104</v>
+      </c>
+      <c r="F7" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="G7" s="36"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
+      <c r="J7" s="37"/>
+      <c r="K7" s="37" t="n">
         <v>2</v>
       </c>
-      <c r="L7" s="39" t="n">
+      <c r="L7" s="37" t="n">
         <v>3</v>
       </c>
-      <c r="M7" s="39" t="n">
+      <c r="M7" s="37" t="n">
         <v>3</v>
       </c>
-      <c r="N7" s="40" t="n">
+      <c r="N7" s="38" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" s="42" t="s">
-        <v>107</v>
-      </c>
-      <c r="F8" s="33" t="s">
-        <v>85</v>
-      </c>
-      <c r="G8" s="38"/>
-      <c r="H8" s="39"/>
-      <c r="I8" s="39" t="n">
+        <v>43</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="F8" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="G8" s="36"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="37" t="n">
         <v>2</v>
       </c>
-      <c r="J8" s="39" t="n">
+      <c r="J8" s="37" t="n">
         <v>2</v>
       </c>
-      <c r="K8" s="39" t="n">
+      <c r="K8" s="37" t="n">
         <v>2</v>
       </c>
-      <c r="L8" s="39" t="n">
+      <c r="L8" s="37" t="n">
         <v>3</v>
       </c>
-      <c r="M8" s="39" t="n">
+      <c r="M8" s="37" t="n">
         <v>3</v>
       </c>
-      <c r="N8" s="40" t="n">
+      <c r="N8" s="38" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="F9" s="33" t="s">
-        <v>85</v>
-      </c>
-      <c r="G9" s="38"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="39" t="n">
+        <v>107</v>
+      </c>
+      <c r="F9" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="G9" s="36"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="37" t="n">
         <v>1</v>
       </c>
-      <c r="J9" s="39" t="n">
+      <c r="J9" s="37" t="n">
         <v>1</v>
       </c>
-      <c r="K9" s="39" t="n">
+      <c r="K9" s="37" t="n">
         <v>1</v>
       </c>
-      <c r="L9" s="39" t="n">
+      <c r="L9" s="37" t="n">
         <v>1</v>
       </c>
-      <c r="M9" s="39" t="n">
+      <c r="M9" s="37" t="n">
         <v>1</v>
       </c>
-      <c r="N9" s="40" t="n">
+      <c r="N9" s="38" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="85.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C10" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="F10" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="G10" s="40"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="41" t="n">
+        <v>2</v>
+      </c>
+      <c r="J10" s="41" t="n">
+        <v>2</v>
+      </c>
+      <c r="K10" s="41" t="n">
+        <v>2</v>
+      </c>
+      <c r="L10" s="41" t="n">
+        <v>2</v>
+      </c>
+      <c r="M10" s="41" t="n">
+        <v>3</v>
+      </c>
+      <c r="N10" s="42" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C10" s="43" t="s">
+      <c r="B11" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C11" s="43" t="s">
         <v>111</v>
-      </c>
-      <c r="F10" s="33" t="s">
-        <v>85</v>
-      </c>
-      <c r="G10" s="44"/>
-      <c r="H10" s="45"/>
-      <c r="I10" s="45" t="n">
-        <v>2</v>
-      </c>
-      <c r="J10" s="45" t="n">
-        <v>2</v>
-      </c>
-      <c r="K10" s="45" t="n">
-        <v>2</v>
-      </c>
-      <c r="L10" s="45" t="n">
-        <v>2</v>
-      </c>
-      <c r="M10" s="45" t="n">
-        <v>3</v>
-      </c>
-      <c r="N10" s="46" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C11" s="47" t="s">
-        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>